<commit_message>
commit code ngày 2020/03/02
</commit_message>
<xml_diff>
--- a/Document/Bài tập training.xlsx
+++ b/Document/Bài tập training.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Team\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuyenNQ\Documents\Trainning202003\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4920868B-0A11-451F-BF9D-6B553A247235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26310" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="4770" yWindow="1320" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LichSu" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>Version No</t>
     <phoneticPr fontId="2"/>
@@ -158,10 +159,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>NV_Nhan</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Trần Thanh Nhân</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -174,81 +171,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>NV_Thanh</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>Hoàng Lê Ph</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ươ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ng Thanh</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>29/04/1988</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>02/10/1995</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>Ph</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ớc Vĩnh, TP Huế</t>
-    </r>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>phuongthanh@gmail.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>0902146977</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>0345245254</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -794,11 +717,78 @@
       <t>ợc thực hiện trên bảng dữ liệu: NhanVienTraining trong CSDL: DBTest</t>
     </r>
   </si>
+  <si>
+    <t>0902146977</t>
+  </si>
+  <si>
+    <t>NV_Thanh</t>
+  </si>
+  <si>
+    <r>
+      <t>Hoàng Lê Ph</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng Thanh</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ph</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ớc Vĩnh, TP Huế</t>
+    </r>
+  </si>
+  <si>
+    <t>phuongthanh@gmail.com</t>
+  </si>
+  <si>
+    <t>0345245254</t>
+  </si>
+  <si>
+    <t>NV_Nhan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -1007,7 +997,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1086,6 +1076,51 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1113,56 +1148,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2 2 2" xfId="2"/>
+    <cellStyle name="標準 2 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1186,7 +1179,7 @@
 </file>
 
 <file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1194,7 +1187,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1256,6 +1249,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1321,6 +1317,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1385,6 +1384,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1439,6 +1441,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1495,6 +1500,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1549,6 +1557,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,6 +1616,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1659,6 +1673,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1715,6 +1732,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2060"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1769,6 +1789,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2061"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1836,6 +1859,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2062"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1901,6 +1927,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2063"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1968,6 +1997,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2064"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2034,6 +2066,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2065"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011080000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2087,7 +2122,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="図 1" descr="Data_NhanVienTraining.PNG"/>
+        <xdr:cNvPr id="2" name="図 1" descr="Data_NhanVienTraining.PNG">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2189,6 +2230,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2224,6 +2282,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2399,7 +2474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -2575,19 +2650,19 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2599,54 +2674,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="28" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="27"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="42"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="28" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1"/>
@@ -2666,23 +2741,23 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="17"/>
@@ -2758,7 +2833,7 @@
     <row r="9" spans="1:21">
       <c r="A9" s="14"/>
       <c r="B9" s="13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -2836,18 +2911,18 @@
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="U12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="14"/>
       <c r="B13" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -2969,7 +3044,7 @@
     <row r="20" spans="1:15">
       <c r="A20" s="14"/>
       <c r="B20" s="13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -3024,173 +3099,173 @@
       <c r="B23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="12" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G23" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="49"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="47" t="s">
+      <c r="H23" s="32"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K23" s="49"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="47" t="s">
+      <c r="K23" s="32"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="48"/>
+      <c r="N23" s="31"/>
       <c r="O23" s="13"/>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="14"/>
       <c r="B24" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
-      <c r="J24" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="K24" s="43"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="N24" s="46"/>
+      <c r="J24" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="36"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24" s="34"/>
       <c r="O24" s="13"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="14"/>
       <c r="B25" s="15" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D25" s="18"/>
-      <c r="E25" s="16" t="s">
-        <v>35</v>
+      <c r="E25" s="50">
+        <v>34740</v>
       </c>
       <c r="F25" s="15"/>
-      <c r="G25" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="43"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N25" s="46"/>
+      <c r="G25" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="39"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25" s="36"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="N25" s="34"/>
       <c r="O25" s="13"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="41"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="3"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="41"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="28"/>
       <c r="O26" s="13"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="41"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="3"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="41"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="28"/>
       <c r="O27" s="13"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="41"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="3"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="41"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="28"/>
       <c r="O28" s="13"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="41"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="3"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="41"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="28"/>
       <c r="O29" s="13"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="41"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="3"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="41"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="28"/>
       <c r="O30" s="13"/>
     </row>
     <row r="31" spans="1:15">
@@ -3211,27 +3286,27 @@
       <c r="O31" s="17"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
+      <c r="A32" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -3250,7 +3325,7 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="17" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -3302,27 +3377,27 @@
       <c r="O36" s="1"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="35"/>
+      <c r="A37" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3358,7 +3433,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3377,7 +3452,7 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3396,7 +3471,7 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3415,7 +3490,7 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3434,7 +3509,7 @@
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3469,27 +3544,27 @@
       <c r="O45" s="1"/>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="35"/>
+      <c r="A46" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3508,7 +3583,7 @@
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3527,7 +3602,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3546,7 +3621,7 @@
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3565,7 +3640,7 @@
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3600,27 +3675,27 @@
       <c r="O52" s="1"/>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="35"/>
+      <c r="A53" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3655,27 +3730,27 @@
       <c r="O55" s="1"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="35"/>
+      <c r="A56" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3710,27 +3785,27 @@
       <c r="O58" s="1"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="35"/>
+      <c r="A59" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="26"/>
+      <c r="N59" s="26"/>
+      <c r="O59" s="26"/>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3765,27 +3840,27 @@
       <c r="O61" s="1"/>
     </row>
     <row r="62" spans="1:15">
-      <c r="A62" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="35"/>
-      <c r="O62" s="35"/>
+      <c r="A62" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="26"/>
+      <c r="N62" s="26"/>
+      <c r="O62" s="26"/>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3804,7 +3879,7 @@
     </row>
     <row r="64" spans="1:15">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3823,7 +3898,7 @@
     </row>
     <row r="65" spans="1:15">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3842,7 +3917,7 @@
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4439,17 +4514,29 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A56:O56"/>
-    <mergeCell ref="A59:O59"/>
-    <mergeCell ref="A62:O62"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A46:O46"/>
-    <mergeCell ref="A53:O53"/>
-    <mergeCell ref="A32:O32"/>
-    <mergeCell ref="A37:O37"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="G23:I23"/>
@@ -4463,34 +4550,22 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="G29:I29"/>
     <mergeCell ref="J29:L29"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="A56:O56"/>
+    <mergeCell ref="A59:O59"/>
+    <mergeCell ref="A62:O62"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="A46:O46"/>
+    <mergeCell ref="A53:O53"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="A37:O37"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="J24" r:id="rId1"/>
-    <hyperlink ref="J25" r:id="rId2"/>
+    <hyperlink ref="J24" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J25" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4499,7 +4574,157 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2065" r:id="rId6" name="TextBox5">
+        <control shapeId="2055" r:id="rId6" name="TextBox1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2055" r:id="rId6" name="TextBox1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2056" r:id="rId8" name="TextBox2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2056" r:id="rId8" name="TextBox2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2057" r:id="rId9" name="TextBox3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>466725</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2057" r:id="rId9" name="TextBox3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2058" r:id="rId10" name="Nam">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>628650</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2058" r:id="rId10" name="Nam"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2059" r:id="rId12" name="Nu">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>781050</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2059" r:id="rId12" name="Nu"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2060" r:id="rId14" name="TextBox4">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>923925</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2060" r:id="rId14" name="TextBox4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2065" r:id="rId16" name="TextBox5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
@@ -4519,157 +4744,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2065" r:id="rId6" name="TextBox5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2060" r:id="rId8" name="TextBox4">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>923925</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2060" r:id="rId8" name="TextBox4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2059" r:id="rId10" name="Nu">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>781050</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2059" r:id="rId10" name="Nu"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2058" r:id="rId12" name="Nam">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>628650</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2058" r:id="rId12" name="Nam"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId14" name="TextBox3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>466725</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2057" r:id="rId14" name="TextBox3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId15" name="TextBox2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2056" r:id="rId15" name="TextBox2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId16" name="TextBox1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2055" r:id="rId16" name="TextBox1"/>
+        <control shapeId="2065" r:id="rId16" name="TextBox5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4831,7 +4906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:Q32"/>
   <sheetViews>
@@ -4846,7 +4921,7 @@
   <sheetData>
     <row r="2" spans="1:17">
       <c r="A2" s="21" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4867,7 +4942,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4888,7 +4963,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="21" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4909,7 +4984,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="21" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4968,7 +5043,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>

</xml_diff>